<commit_message>
project CG complete Branching to be completed
</commit_message>
<xml_diff>
--- a/TIF/results.xlsx
+++ b/TIF/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skema-my.sharepoint.com/personal/morteza_davari_skema_edu/Documents/Data/Research/1- OnGoing/Graph - Balanced Tree/Heavest Balanced Tree/TIF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22070D3A-E59A-4320-9519-B82B7FDE5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{22070D3A-E59A-4320-9519-B82B7FDE5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F85132F6-8458-4171-97FD-E141A5BF8429}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{6A9E7A66-5590-44F5-BA66-18E77DB9A2F0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{6A9E7A66-5590-44F5-BA66-18E77DB9A2F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D86A0D-3B16-4799-B18E-88C3DABA20D5}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D86A0D-3B16-4799-B18E-88C3DABA20D5}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C20" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="2">
     <pivotField numFmtId="2" showAll="0"/>
@@ -711,94 +711,94 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -813,12 +813,15 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -914,7 +917,7 @@
         <v>20.952380952380953</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -953,7 +956,7 @@
         <v>0.57258064516128526</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="L3:M13" si="2">($F3-H3)/$F3*100</f>
+        <f t="shared" ref="M3:M13" si="2">($F3-H3)/$F3*100</f>
         <v>0</v>
       </c>
       <c r="N3" s="1">
@@ -975,7 +978,7 @@
         <v>45.967741935483872</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>59.433962264150942</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>76.923076923076934</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>34.45378151260504</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>45.333333333333329</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>55.555555555555557</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>60.416666666666664</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>39.705882352941174</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>66.071428571428569</v>
       </c>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>12</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>13</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>14</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
         <v>15</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>16</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>17</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>18</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>19</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
         <v>20</v>
       </c>
@@ -1905,7 +1908,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
         <v>21</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
         <v>22</v>
       </c>
@@ -1975,4 +1978,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{9860db96-b53f-4bd7-8137-e09357cab268}" enabled="1" method="Standard" siteId="{b78d03e6-f6a2-4cff-83be-847d1a6453f9}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>